<commit_message>
Added roles to Role-Front
</commit_message>
<xml_diff>
--- a/Cards/RoleData/Role-Front.xlsx
+++ b/Cards/RoleData/Role-Front.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tech\Github Repos\TEAM-TEAM-TraitorCards\Cards\RoleData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACA67DEB-174F-475C-9A57-8ED585256169}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B137C37-3285-4E22-8D53-3B8578756DF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1E0E38A4-A720-4B05-94AE-F55473173966}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
   <si>
     <t>Name</t>
   </si>
@@ -62,7 +62,42 @@
     <t>KingEffectText</t>
   </si>
   <si>
-    <t>AbilityText</t>
+    <t>King</t>
+  </si>
+  <si>
+    <t>Traitor</t>
+  </si>
+  <si>
+    <t>Loyalist</t>
+  </si>
+  <si>
+    <t>King.ai</t>
+  </si>
+  <si>
+    <t>Traitor.ai</t>
+  </si>
+  <si>
+    <t>Loyalist.ai</t>
+  </si>
+  <si>
+    <t>Heart.ai</t>
+  </si>
+  <si>
+    <t>Damage.ai</t>
+  </si>
+  <si>
+    <t>Protection.ai</t>
+  </si>
+  <si>
+    <t>x2 to king, if alive.</t>
+  </si>
+  <si>
+    <t>FavourText</t>
+  </si>
+  <si>
+    <t>Once per game:
+- Peek at a players role OR
+- Move a Delegate between Courts</t>
   </si>
 </sst>
 </file>
@@ -112,13 +147,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -454,10 +498,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81838662-B590-45E0-82FF-5E356D98D8D1}">
-  <dimension ref="A1:K20"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -465,10 +509,10 @@
     <col min="1" max="1" width="28.7109375" customWidth="1"/>
     <col min="2" max="2" width="30.85546875" customWidth="1"/>
     <col min="3" max="6" width="19" customWidth="1"/>
-    <col min="7" max="13" width="32.85546875" customWidth="1"/>
+    <col min="7" max="9" width="32.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -494,30 +538,84 @@
         <v>7</v>
       </c>
       <c r="I1" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
+      <c r="B2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="5" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="2" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="17" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="18" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Created icky dev template for Roles
</commit_message>
<xml_diff>
--- a/Cards/RoleData/Role-Front.xlsx
+++ b/Cards/RoleData/Role-Front.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tech\Github Repos\TEAM-TEAM-TraitorCards\Cards\RoleData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B137C37-3285-4E22-8D53-3B8578756DF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2443A1A-6FA8-4779-9E45-4B3A6FEB8ACC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1E0E38A4-A720-4B05-94AE-F55473173966}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
   <si>
     <t>Name</t>
   </si>
@@ -98,6 +98,12 @@
     <t>Once per game:
 - Peek at a players role OR
 - Move a Delegate between Courts</t>
+  </si>
+  <si>
+    <t>VictoryText</t>
+  </si>
+  <si>
+    <t>Wins if alive.</t>
   </si>
 </sst>
 </file>
@@ -498,10 +504,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81838662-B590-45E0-82FF-5E356D98D8D1}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -510,9 +516,10 @@
     <col min="2" max="2" width="30.85546875" customWidth="1"/>
     <col min="3" max="6" width="19" customWidth="1"/>
     <col min="7" max="9" width="32.85546875" customWidth="1"/>
+    <col min="10" max="10" width="32.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -532,16 +539,19 @@
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
@@ -560,13 +570,16 @@
       <c r="F2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="4"/>
+      <c r="G2" s="4" t="s">
+        <v>21</v>
+      </c>
       <c r="H2" s="4"/>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="4"/>
+      <c r="J2" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
@@ -581,17 +594,18 @@
         <v>14</v>
       </c>
       <c r="F3" s="4"/>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="4"/>
+      <c r="H3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="I3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="J3" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
@@ -606,13 +620,14 @@
         <v>14</v>
       </c>
       <c r="F4" s="4"/>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="4"/>
+      <c r="H4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="I4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="J4" s="5" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Sideways Role cards done
</commit_message>
<xml_diff>
--- a/Cards/RoleData/Role-Front.xlsx
+++ b/Cards/RoleData/Role-Front.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tech\Github Repos\TEAM-TEAM-TraitorCards\Cards\RoleData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8FE79F3-BEB3-4BC2-A42F-EC3A948CD4F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB19B785-10D7-4CD0-A2E9-983760D68C6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-1290" windowWidth="29040" windowHeight="15840" xr2:uid="{1E0E38A4-A720-4B05-94AE-F55473173966}"/>
   </bookViews>
@@ -65,15 +65,6 @@
     <t>Loyalist</t>
   </si>
   <si>
-    <t>King.ai</t>
-  </si>
-  <si>
-    <t>Traitor.ai</t>
-  </si>
-  <si>
-    <t>Loyalist.ai</t>
-  </si>
-  <si>
     <t>Heart.ai</t>
   </si>
   <si>
@@ -96,6 +87,15 @@
   </si>
   <si>
     <t>2 HP</t>
+  </si>
+  <si>
+    <t>King.png</t>
+  </si>
+  <si>
+    <t>Traitor.png</t>
+  </si>
+  <si>
+    <t>Loyalist.png</t>
   </si>
 </sst>
 </file>
@@ -499,7 +499,7 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -530,10 +530,10 @@
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -541,25 +541,25 @@
         <v>6</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -567,20 +567,20 @@
         <v>7</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="C3" s="4"/>
       <c r="E3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="5" t="s">
         <v>12</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -588,20 +588,20 @@
         <v>8</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="C4" s="4"/>
       <c r="E4" s="4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>